<commit_message>
adding NA to lookup table and adjusting enums accordingly
</commit_message>
<xml_diff>
--- a/nbs/files/lut/dbo_area.xlsx
+++ b/nbs/files/lut/dbo_area.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/franckalbinet/pro/IAEA/MARIS/marisco/nbs/files/lut/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8C2D368-80DC-0948-A501-E72258CAB655}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80535206-D896-644F-8C08-19B1FDA6510C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="128">
   <si>
     <t>areaId</t>
   </si>
@@ -399,13 +399,19 @@
   </si>
   <si>
     <t>Unassigned</t>
+  </si>
+  <si>
+    <t>Not available</t>
+  </si>
+  <si>
+    <t>Not applicable</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -415,6 +421,11 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -455,10 +466,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -762,16 +785,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B132"/>
+  <dimension ref="A1:B134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
-      <selection activeCell="B107" sqref="B107"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47" customWidth="1"/>
+    <col min="2" max="2" width="36.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -783,1050 +806,1066 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
+      <c r="A2" s="4">
+        <v>-1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
+      <c r="A3" s="2">
+        <v>0</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="B19" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B20" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B21" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="B22" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B23" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B24" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="B25" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="B26" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="B27" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="B28" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="B29" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="B30" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>1904</v>
+        <v>87</v>
       </c>
       <c r="B31" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>1906</v>
+        <v>88</v>
       </c>
       <c r="B32" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>1907</v>
+        <v>1904</v>
       </c>
       <c r="B33" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>1908</v>
+        <v>1906</v>
       </c>
       <c r="B34" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>1910</v>
+        <v>1907</v>
       </c>
       <c r="B35" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>1912</v>
+        <v>1908</v>
       </c>
       <c r="B36" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>1914</v>
+        <v>1910</v>
       </c>
       <c r="B37" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>2350</v>
+        <v>1912</v>
       </c>
       <c r="B38" t="s">
-        <v>31</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>2351</v>
+        <v>1914</v>
       </c>
       <c r="B39" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>2353</v>
+        <v>2350</v>
       </c>
       <c r="B40" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>2356</v>
+        <v>2351</v>
       </c>
       <c r="B41" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>2357</v>
+        <v>2353</v>
       </c>
       <c r="B42" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>2359</v>
+        <v>2356</v>
       </c>
       <c r="B43" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>2374</v>
+        <v>2357</v>
       </c>
       <c r="B44" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45">
-        <v>2379</v>
+        <v>2359</v>
       </c>
       <c r="B45" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46">
-        <v>2389</v>
+        <v>2374</v>
       </c>
       <c r="B46" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>2401</v>
+        <v>2379</v>
       </c>
       <c r="B47" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48">
-        <v>2402</v>
+        <v>2389</v>
       </c>
       <c r="B48" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49">
-        <v>2407</v>
+        <v>2401</v>
       </c>
       <c r="B49" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50">
-        <v>2409</v>
+        <v>2402</v>
       </c>
       <c r="B50" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51">
-        <v>3141</v>
+        <v>2407</v>
       </c>
       <c r="B51" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52">
-        <v>3314</v>
+        <v>2409</v>
       </c>
       <c r="B52" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53">
-        <v>3315</v>
+        <v>3141</v>
       </c>
       <c r="B53" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54">
-        <v>3319</v>
+        <v>3314</v>
       </c>
       <c r="B54" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55">
-        <v>3320</v>
+        <v>3315</v>
       </c>
       <c r="B55" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56">
-        <v>3322</v>
+        <v>3319</v>
       </c>
       <c r="B56" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57">
-        <v>3324</v>
+        <v>3320</v>
       </c>
       <c r="B57" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58">
-        <v>3346</v>
+        <v>3322</v>
       </c>
       <c r="B58" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59">
-        <v>3351</v>
+        <v>3324</v>
       </c>
       <c r="B59" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60">
-        <v>3363</v>
+        <v>3346</v>
       </c>
       <c r="B60" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61">
-        <v>3369</v>
+        <v>3351</v>
       </c>
       <c r="B61" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62">
-        <v>3386</v>
+        <v>3363</v>
       </c>
       <c r="B62" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63">
-        <v>4244</v>
+        <v>3369</v>
       </c>
       <c r="B63" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64">
-        <v>4245</v>
+        <v>3386</v>
       </c>
       <c r="B64" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65">
-        <v>4246</v>
+        <v>4244</v>
       </c>
       <c r="B65" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66">
-        <v>4247</v>
+        <v>4245</v>
       </c>
       <c r="B66" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67">
-        <v>4248</v>
+        <v>4246</v>
       </c>
       <c r="B67" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68">
-        <v>4250</v>
+        <v>4247</v>
       </c>
       <c r="B68" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69">
-        <v>4251</v>
+        <v>4248</v>
       </c>
       <c r="B69" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70">
-        <v>4252</v>
+        <v>4250</v>
       </c>
       <c r="B70" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71">
-        <v>4253</v>
+        <v>4251</v>
       </c>
       <c r="B71" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72">
-        <v>4254</v>
+        <v>4252</v>
       </c>
       <c r="B72" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73">
-        <v>4256</v>
+        <v>4253</v>
       </c>
       <c r="B73" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74">
-        <v>4257</v>
+        <v>4254</v>
       </c>
       <c r="B74" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75">
-        <v>4261</v>
+        <v>4256</v>
       </c>
       <c r="B75" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76">
-        <v>4262</v>
+        <v>4257</v>
       </c>
       <c r="B76" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77">
-        <v>4263</v>
+        <v>4261</v>
       </c>
       <c r="B77" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78">
-        <v>4264</v>
+        <v>4262</v>
       </c>
       <c r="B78" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79">
-        <v>4265</v>
+        <v>4263</v>
       </c>
       <c r="B79" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80">
-        <v>4266</v>
+        <v>4264</v>
       </c>
       <c r="B80" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81">
-        <v>4267</v>
+        <v>4265</v>
       </c>
       <c r="B81" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82">
-        <v>4268</v>
+        <v>4266</v>
       </c>
       <c r="B82" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83">
-        <v>4269</v>
+        <v>4267</v>
       </c>
       <c r="B83" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84">
-        <v>4273</v>
+        <v>4268</v>
       </c>
       <c r="B84" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85">
-        <v>4274</v>
+        <v>4269</v>
       </c>
       <c r="B85" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86">
-        <v>4275</v>
+        <v>4273</v>
       </c>
       <c r="B86" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87">
-        <v>4276</v>
+        <v>4274</v>
       </c>
       <c r="B87" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88">
-        <v>4279</v>
+        <v>4275</v>
       </c>
       <c r="B88" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89">
-        <v>4280</v>
+        <v>4276</v>
       </c>
       <c r="B89" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90">
-        <v>4283</v>
+        <v>4279</v>
       </c>
       <c r="B90" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91">
-        <v>4286</v>
+        <v>4280</v>
       </c>
       <c r="B91" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92">
-        <v>4287</v>
+        <v>4283</v>
       </c>
       <c r="B92" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93">
-        <v>4288</v>
+        <v>4286</v>
       </c>
       <c r="B93" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94">
-        <v>4289</v>
+        <v>4287</v>
       </c>
       <c r="B94" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95">
-        <v>4290</v>
+        <v>4288</v>
       </c>
       <c r="B95" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96">
-        <v>4291</v>
+        <v>4289</v>
       </c>
       <c r="B96" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97">
-        <v>4300</v>
+        <v>4290</v>
       </c>
       <c r="B97" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98">
-        <v>4302</v>
+        <v>4291</v>
       </c>
       <c r="B98" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99">
-        <v>4303</v>
+        <v>4300</v>
       </c>
       <c r="B99" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100">
-        <v>4306</v>
+        <v>4302</v>
       </c>
       <c r="B100" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101">
-        <v>4307</v>
+        <v>4303</v>
       </c>
       <c r="B101" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102">
-        <v>4309</v>
+        <v>4306</v>
       </c>
       <c r="B102" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103">
-        <v>4310</v>
+        <v>4307</v>
       </c>
       <c r="B103" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104">
-        <v>4312</v>
+        <v>4309</v>
       </c>
       <c r="B104" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105">
-        <v>4313</v>
+        <v>4310</v>
       </c>
       <c r="B105" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106">
-        <v>4314</v>
+        <v>4312</v>
       </c>
       <c r="B106" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107">
-        <v>4325</v>
+        <v>4313</v>
       </c>
       <c r="B107" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108">
-        <v>4332</v>
+        <v>4314</v>
       </c>
       <c r="B108" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109">
-        <v>4334</v>
+        <v>4325</v>
       </c>
       <c r="B109" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A110">
-        <v>4336</v>
+        <v>4332</v>
       </c>
       <c r="B110" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A111">
-        <v>4338</v>
+        <v>4334</v>
       </c>
       <c r="B111" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A112">
-        <v>4339</v>
+        <v>4336</v>
       </c>
       <c r="B112" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A113">
-        <v>4340</v>
+        <v>4338</v>
       </c>
       <c r="B113" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A114">
-        <v>4341</v>
+        <v>4339</v>
       </c>
       <c r="B114" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A115">
-        <v>4343</v>
+        <v>4340</v>
       </c>
       <c r="B115" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A116">
-        <v>4344</v>
+        <v>4341</v>
       </c>
       <c r="B116" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A117">
-        <v>4347</v>
+        <v>4343</v>
       </c>
       <c r="B117" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A118">
-        <v>4349</v>
+        <v>4344</v>
       </c>
       <c r="B118" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A119">
-        <v>4350</v>
+        <v>4347</v>
       </c>
       <c r="B119" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A120">
-        <v>4351</v>
+        <v>4349</v>
       </c>
       <c r="B120" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A121">
-        <v>4353</v>
+        <v>4350</v>
       </c>
       <c r="B121" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A122">
-        <v>4354</v>
+        <v>4351</v>
       </c>
       <c r="B122" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A123">
-        <v>4355</v>
+        <v>4353</v>
       </c>
       <c r="B123" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A124">
-        <v>4358</v>
+        <v>4354</v>
       </c>
       <c r="B124" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A125">
-        <v>4359</v>
+        <v>4355</v>
       </c>
       <c r="B125" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A126">
-        <v>4360</v>
+        <v>4358</v>
       </c>
       <c r="B126" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A127">
-        <v>4361</v>
+        <v>4359</v>
       </c>
       <c r="B127" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A128">
-        <v>4364</v>
+        <v>4360</v>
       </c>
       <c r="B128" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A129">
-        <v>4365</v>
+        <v>4361</v>
       </c>
       <c r="B129" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A130">
-        <v>4366</v>
+        <v>4364</v>
       </c>
       <c r="B130" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A131">
-        <v>5698</v>
+        <v>4365</v>
       </c>
       <c r="B131" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A132">
+        <v>4366</v>
+      </c>
+      <c r="B132" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A133">
+        <v>5698</v>
+      </c>
+      <c r="B133" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A134">
         <v>9999</v>
       </c>
-      <c r="B132" t="s">
+      <c r="B134" t="s">
         <v>125</v>
       </c>
     </row>

</xml_diff>